<commit_message>
A bunch of minor changes in several scripts.
</commit_message>
<xml_diff>
--- a/data-raw/regions lookup Sep 6 2016.xlsx
+++ b/data-raw/regions lookup Sep 6 2016.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="15960"/>
+    <workbookView xWindow="41020" yWindow="140" windowWidth="28800" windowHeight="15960" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="dt.regions.all" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7653" uniqueCount="1210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7654" uniqueCount="1211">
   <si>
     <t>ISO_code</t>
   </si>
@@ -3672,6 +3672,9 @@
   </si>
   <si>
     <t>region.code</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -3735,12 +3738,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3886,6 +3891,9 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -3894,9 +3902,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3946,7 +3951,7 @@
     <tableColumn id="1" name="ISO_code"/>
     <tableColumn id="17" name="region_name.AggReg2"/>
     <tableColumn id="18" name="region_code.AggReg2"/>
-    <tableColumn id="2" name="region_code.AggReg3" dataDxfId="1">
+    <tableColumn id="2" name="region_code.AggReg3" dataDxfId="0">
       <calculatedColumnFormula>VLOOKUP(A2,ISO!$A$2:'ISO'!$D$251,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="region_code.AggReg4"/>
@@ -4236,7 +4241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
@@ -34999,8 +35004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K251"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35105,6 +35110,9 @@
       </c>
       <c r="D6" t="e">
         <v>#N/A</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1210</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -53352,7 +53360,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>